<commit_message>
carga masiva de consumo, incluyendo solicitante y area
</commit_message>
<xml_diff>
--- a/assets/files/plantilla_de_carga_NI.xlsx
+++ b/assets/files/plantilla_de_carga_NI.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\overlap09\Desktop\modulos\ROCKDRILL\almacenes-virtualesv2\assets\files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Aplicaciones\Rockdrill\Almacenes Virtuales VPS- Logistica\assets\files\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,8 +23,123 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>user</author>
+  </authors>
+  <commentList>
+    <comment ref="A1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Obligatorio
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">En caso de no tener serie dejar en blanco, evitar espacios en blanco
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Obligatorio</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Campo opcional, tener en cuenta las maquinas registradas en el contrato escribiendo el NOMBRE, de caso contrario validara con un error.
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Opcional. Para no tener inconvenientes en el reporte por vales escribir de la siguiente manera
+(VS N° 066174) respetando los espacios</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>CAMPO OPCIONAL,
+INDICAR EL NUMERO DE SOLICITANTE CON EL QUE SE REGISTRO EN LA APLICACIÓN,DE LO CONTRARIO NO REGISTRARA EL CONSUMO</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">Campo opcional,
+Indicar el numero asignado al area en el aplicativo para evitar errores
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>CODIGO</t>
   </si>
@@ -39,19 +154,32 @@
   </si>
   <si>
     <t>DOCREF</t>
+  </si>
+  <si>
+    <t>SOLICITANTE</t>
+  </si>
+  <si>
+    <t>AREA</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -358,14 +486,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.5703125" customWidth="1"/>
+    <col min="2" max="2" width="23.42578125" customWidth="1"/>
+    <col min="3" max="3" width="29.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" customWidth="1"/>
+    <col min="5" max="5" width="22.28515625" customWidth="1"/>
+    <col min="6" max="6" width="14.5703125" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
@@ -383,8 +519,12 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
@@ -416,5 +556,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>